<commit_message>
Changed formating on example sheet
</commit_message>
<xml_diff>
--- a/Python Agent Master Sheet.xlsx
+++ b/Python Agent Master Sheet.xlsx
@@ -840,7 +840,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1233,7 +1233,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1353,12 +1353,15 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="1" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="17.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>